<commit_message>
custom user profil, add tweet
</commit_message>
<xml_diff>
--- a/pontozas.xlsx
+++ b/pontozas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Suli\Files\Webfejlesztes\fake_twitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B16A97F-0223-4D55-BB06-7AC9BC5429CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0295EC5B-9692-48BA-B986-CA36FF83C3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C023ABD7-0EEF-4DA5-90CE-1E10D46CB121}"/>
   </bookViews>
@@ -601,7 +601,7 @@
   <dimension ref="B1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,13 +659,13 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="3"/>
@@ -673,14 +673,14 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="2:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+    <row r="6" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3"/>
@@ -851,14 +851,14 @@
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="2:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+    <row r="18" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C18" s="6">
+        <v>1</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E18" s="3"/>
@@ -896,14 +896,14 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="2:8" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="2:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="6">
         <v>2</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E21" s="3"/>

</xml_diff>